<commit_message>
Addition on TestSuite excel file
- New lead creation test cases added
- Objectrepository updated with xpaths
- selectItem() method added to Keywords class

Signed-off-by: Renju Jose <renjujv@gmail.com>
</commit_message>
<xml_diff>
--- a/res/TestSuite.xlsx
+++ b/res/TestSuite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Description</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Click on leads link</t>
   </si>
   <si>
-    <t>Clck on new button</t>
-  </si>
-  <si>
     <t>Enter Last Name</t>
   </si>
   <si>
@@ -63,12 +60,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>testusername</t>
-  </si>
-  <si>
-    <t>testpassword</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -124,6 +115,57 @@
   </si>
   <si>
     <t>selectorname</t>
+  </si>
+  <si>
+    <t>Select Lead status</t>
+  </si>
+  <si>
+    <t>Select Name salutation</t>
+  </si>
+  <si>
+    <t>Enter Company Name</t>
+  </si>
+  <si>
+    <t>Click on Save button</t>
+  </si>
+  <si>
+    <t>Click on new button</t>
+  </si>
+  <si>
+    <t>selectItem</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>leadstatselector</t>
+  </si>
+  <si>
+    <t>namesalutselector</t>
+  </si>
+  <si>
+    <t>firstnametextbox</t>
+  </si>
+  <si>
+    <t>lastnametextbox</t>
+  </si>
+  <si>
+    <t>companytextbox</t>
+  </si>
+  <si>
+    <t>savebutton</t>
+  </si>
+  <si>
+    <t>Sutherland</t>
+  </si>
+  <si>
+    <t>lavanya.kpv@gmail.com</t>
+  </si>
+  <si>
+    <t>kavilputhenlavu1</t>
   </si>
 </sst>
 </file>
@@ -523,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +578,7 @@
     <col min="3" max="3" width="15" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19" style="3" customWidth="1"/>
     <col min="7" max="7" width="11" style="3" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
@@ -549,22 +591,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -575,16 +617,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G2" s="2" t="b">
         <v>1</v>
@@ -601,16 +643,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="b">
         <v>1</v>
@@ -627,22 +669,22 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,22 +695,22 @@
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -679,22 +721,22 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,22 +747,22 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -731,22 +773,22 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,25 +796,25 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -780,25 +822,25 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -806,33 +848,138 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="b">
-        <v>1</v>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>